<commit_message>
Baseline updates: - Bigbird baseline created - Updated all baseline for comparison - Compare all of the baselines with the same test data and document it in the excel
</commit_message>
<xml_diff>
--- a/DataScrape/Summary.xlsx
+++ b/DataScrape/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmeedu-my.sharepoint.com/personal/olah_bence_edu_bme_hu/Documents/BME/MSc/Diplomatéma/StockMarketSentimentAnalysis/DataScrape/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="320" documentId="8_{286F456F-0092-482B-B7E3-20BF2E9602AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{95E9DC52-0A98-4E1A-A7ED-F4E11910EDEB}"/>
+  <xr:revisionPtr revIDLastSave="324" documentId="8_{286F456F-0092-482B-B7E3-20BF2E9602AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3F22C426-9D3D-48A3-A38C-D96E4813A01C}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B1D3D369-B0C5-4482-B75C-AA467DDE30B8}"/>
   </bookViews>
@@ -499,16 +499,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
@@ -517,47 +514,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Palatino Linotype"/>
-        <family val="1"/>
-        <charset val="238"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -915,13 +881,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -956,6 +915,48 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Palatino Linotype"/>
+        <family val="1"/>
+        <charset val="238"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -970,18 +971,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9DC63B21-3316-424A-A76D-3DA78C6936DC}" name="Table1" displayName="Table1" ref="A1:I23" totalsRowShown="0" headerRowDxfId="0" dataDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9DC63B21-3316-424A-A76D-3DA78C6936DC}" name="Table1" displayName="Table1" ref="A1:I23" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A1:I23" xr:uid="{4B1CD4D6-11B8-4C40-927F-F737D6B3D4CD}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{013BB50D-1796-426B-83E8-1B208CD019C0}" name="Group" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{DD4B7C85-49A7-41B5-A016-1FF6BB762B91}" name="Name" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{DA405F4F-A92C-403D-AC53-7DDF629DEAC2}" name="Source" dataDxfId="7" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" xr3:uid="{0E251E1F-0871-48BB-9172-533967D77D78}" name="Type" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{7B7D9AD4-8C29-4AD2-B6FE-A9C8183542BD}" name="Date From" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{E25A4B2F-B837-4EC0-9056-54C37D6179AB}" name="Date To" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{8E7A5488-FDA3-4BB2-907E-E45103F6A920}" name="Quantity" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{A619206E-B230-4E20-BA42-382C6B4BA1DB}" name="Size" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{3425F2BF-651E-49D9-925B-CD66A4700E24}" name="Preprocess before upload" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{013BB50D-1796-426B-83E8-1B208CD019C0}" name="Group" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{DD4B7C85-49A7-41B5-A016-1FF6BB762B91}" name="Name" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{DA405F4F-A92C-403D-AC53-7DDF629DEAC2}" name="Source" dataDxfId="6" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" xr3:uid="{0E251E1F-0871-48BB-9172-533967D77D78}" name="Type" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{7B7D9AD4-8C29-4AD2-B6FE-A9C8183542BD}" name="Date From" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{E25A4B2F-B837-4EC0-9056-54C37D6179AB}" name="Date To" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{8E7A5488-FDA3-4BB2-907E-E45103F6A920}" name="Quantity" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{A619206E-B230-4E20-BA42-382C6B4BA1DB}" name="Size" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{3425F2BF-651E-49D9-925B-CD66A4700E24}" name="Preprocess before upload" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1286,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E116FF82-8D87-48AC-AA35-F370C7C8BC1B}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,16 +1340,16 @@
       <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>35495</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>44240</v>
       </c>
       <c r="G2" s="5">
@@ -1357,7 +1358,7 @@
       <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1368,16 +1369,16 @@
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="14" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>11130</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>44235</v>
       </c>
       <c r="G3" s="5">
@@ -1386,7 +1387,7 @@
       <c r="H3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1397,16 +1398,16 @@
       <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="14" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>25543</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>44254</v>
       </c>
       <c r="G4" s="5">
@@ -1415,7 +1416,7 @@
       <c r="H4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1426,16 +1427,16 @@
       <c r="B5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>42771</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>44253</v>
       </c>
       <c r="G5" s="5">
@@ -1444,7 +1445,7 @@
       <c r="H5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1455,16 +1456,16 @@
       <c r="B6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="6">
         <v>41002</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <v>44238</v>
       </c>
       <c r="G6" s="5">
@@ -1473,7 +1474,7 @@
       <c r="H6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1484,16 +1485,16 @@
       <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8" t="s">
         <v>31</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="6">
         <v>43897</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="6">
         <v>44253</v>
       </c>
       <c r="G7" s="5">
@@ -1502,7 +1503,7 @@
       <c r="H7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1513,16 +1514,16 @@
       <c r="B8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>44140</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>44253</v>
       </c>
       <c r="G8" s="5">
@@ -1531,7 +1532,7 @@
       <c r="H8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1542,16 +1543,16 @@
       <c r="B9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>37</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>43760</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>44253</v>
       </c>
       <c r="G9" s="5">
@@ -1560,7 +1561,7 @@
       <c r="H9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I9" s="8" t="s">
+      <c r="I9" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1571,16 +1572,16 @@
       <c r="B10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>44</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>43111</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>44253</v>
       </c>
       <c r="G10" s="5">
@@ -1589,7 +1590,7 @@
       <c r="H10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1600,16 +1601,16 @@
       <c r="B11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>48</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>43409</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>44236</v>
       </c>
       <c r="G11" s="5">
@@ -1618,7 +1619,7 @@
       <c r="H11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="I11" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1629,16 +1630,16 @@
       <c r="B12" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>54</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>42601</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>44254</v>
       </c>
       <c r="G12" s="5">
@@ -1647,7 +1648,7 @@
       <c r="H12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1658,16 +1659,16 @@
       <c r="B13" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>56</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <v>43937</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>44254</v>
       </c>
       <c r="G13" s="5">
@@ -1676,7 +1677,7 @@
       <c r="H13" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1687,16 +1688,16 @@
       <c r="B14" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="14" t="s">
         <v>60</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <v>39668</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="6">
         <v>42552</v>
       </c>
       <c r="G14" s="5">
@@ -1705,7 +1706,7 @@
       <c r="H14" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1716,16 +1717,16 @@
       <c r="B15" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>63</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <v>39052</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>41416</v>
       </c>
       <c r="G15" s="5">
@@ -1734,7 +1735,7 @@
       <c r="H15" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I15" s="8" t="s">
+      <c r="I15" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1745,16 +1746,16 @@
       <c r="B16" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="8" t="s">
         <v>63</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <v>39052</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="6">
         <v>42704</v>
       </c>
       <c r="G16" s="5">
@@ -1763,7 +1764,7 @@
       <c r="H16" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="I16" s="8" t="s">
+      <c r="I16" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1774,16 +1775,16 @@
       <c r="B17" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="8" t="s">
         <v>71</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>40675</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>43987</v>
       </c>
       <c r="G17" s="5">
@@ -1792,7 +1793,7 @@
       <c r="H17" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I17" s="8" t="s">
+      <c r="I17" s="7" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1803,16 +1804,16 @@
       <c r="B18" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>71</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>40948</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <v>43983</v>
       </c>
       <c r="G18" s="5">
@@ -1821,7 +1822,7 @@
       <c r="H18" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="I18" s="8" t="s">
+      <c r="I18" s="7" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1832,16 +1833,16 @@
       <c r="B19" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>43091</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>44029</v>
       </c>
       <c r="G19" s="5">
@@ -1850,7 +1851,7 @@
       <c r="H19" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="I19" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1861,16 +1862,16 @@
       <c r="B20" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>43086</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>44030</v>
       </c>
       <c r="G20" s="5">
@@ -1879,7 +1880,7 @@
       <c r="H20" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="I20" s="8" t="s">
+      <c r="I20" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1890,16 +1891,16 @@
       <c r="B21" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>81</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>43179</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>44030</v>
       </c>
       <c r="G21" s="5">
@@ -1908,7 +1909,7 @@
       <c r="H21" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1919,16 +1920,16 @@
       <c r="B22" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>40908</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="6">
         <v>43845</v>
       </c>
       <c r="G22" s="5">
@@ -1937,36 +1938,36 @@
       <c r="H22" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I22" s="7" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="12">
         <v>42005</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="12">
         <v>43830</v>
       </c>
-      <c r="G23" s="11">
+      <c r="G23" s="10">
         <v>4336445</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="H23" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="13" t="s">
         <v>76</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Baseline updates: - New twitter dataset work with -.- VADER -.- logreg -.- LSTM
</commit_message>
<xml_diff>
--- a/DataScrape/Summary.xlsx
+++ b/DataScrape/Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bmeedu-my.sharepoint.com/personal/olah_bence_edu_bme_hu/Documents/BME/MSc/Diplomatéma/StockMarketSentimentAnalysis/DataScrape/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="324" documentId="8_{286F456F-0092-482B-B7E3-20BF2E9602AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3F22C426-9D3D-48A3-A38C-D96E4813A01C}"/>
+  <xr:revisionPtr revIDLastSave="325" documentId="8_{286F456F-0092-482B-B7E3-20BF2E9602AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8D59A78E-35C6-47A1-B2EC-CF27E884507B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B1D3D369-B0C5-4482-B75C-AA467DDE30B8}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B1D3D369-B0C5-4482-B75C-AA467DDE30B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1287,24 +1287,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E116FF82-8D87-48AC-AA35-F370C7C8BC1B}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17:G18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="98.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
@@ -1536,7 +1536,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>46</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>46</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>46</v>
       </c>
@@ -1681,7 +1681,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>59</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>59</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>59</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>59</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>59</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>59</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>59</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>59</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>59</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>59</v>
       </c>

</xml_diff>